<commit_message>
updated feedback form for dairy_digester, excel compare, and excel_macros
</commit_message>
<xml_diff>
--- a/feedback_forms/processed_versions/xl_workbooks/dairy_digester_operator_feedback_v005.xlsx
+++ b/feedback_forms/processed_versions/xl_workbooks/dairy_digester_operator_feedback_v005.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\current_versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tony_local\pycharm\feedback_portal\feedback_forms\processed_versions\xl_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB31801-DD57-4FF2-ACFD-45F737648F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C28075-EF69-480A-9929-7666018583E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3993" yWindow="733" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
+    <workbookView xWindow="3553" yWindow="1613" windowWidth="19200" windowHeight="11387" tabRatio="705" xr2:uid="{908CDDAE-4CC3-4DCD-AAA9-A26C259C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedback Form" sheetId="6" r:id="rId1"/>
@@ -84,7 +84,7 @@
     <definedName name="jinja_transport_recipient">'Feedback Form'!$D$92</definedName>
     <definedName name="jinji_transport_recipient">'Feedback Form'!$D$92</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3641,8 +3641,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -8508,26 +8508,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E9A34E7C7C736409D4BDE6375CCC276" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cf521a6d855790dbe6a6d894ff439cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32" xmlns:ns3="e20ceb87-0d79-402a-b4b9-75d78589c76d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45aa6d812898c4b0f52b4c3685679ce" ns2:_="" ns3:_="">
     <xsd:import namespace="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
@@ -8762,26 +8742,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
-    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e20ceb87-0d79-402a-b4b9-75d78589c76d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC83B422-5B73-4269-9006-1DDE9C149499}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8800,6 +8781,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393EEAE4-A9A0-45DD-A8E7-CAAABB0BE8BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567EEBE1-6545-4ECC-A20C-42A5CA5522CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1aa5fbe9-a248-4c55-92b7-8f3861f8fb32"/>
+    <ds:schemaRef ds:uri="e20ceb87-0d79-402a-b4b9-75d78589c76d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" enabled="0" method="" siteId="{9de5aaee-7788-40b1-a438-c0ccc98c87cc}" removed="1"/>

</xml_diff>